<commit_message>
Preparing all for deployment
</commit_message>
<xml_diff>
--- a/04_project/calculo_tiempo_esfuerzo_productividad.xlsx
+++ b/04_project/calculo_tiempo_esfuerzo_productividad.xlsx
@@ -149,11 +149,11 @@
   </sheetPr>
   <dimension ref="E8:F24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.17"/>
   </cols>

</xml_diff>